<commit_message>
correction for walameni. Service, test and file is changed
</commit_message>
<xml_diff>
--- a/data/crac-file/crac-file-xlsx-api/src/test/resources/test_crac_simple.xlsx
+++ b/data/crac-file/crac-file-xlsx-api/src/test/resources/test_crac_simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">Penalty Cost Tap Change (EUR/Delta tap h)</t>
   </si>
   <si>
-    <t xml:space="preserve">Penalty costs for absolute difference between tap positions of two time steps (gradients of tap position --&gt;Smooting the initial sequence _x005F_x005F_x005F_x005F_x000B_of tap positions</t>
+    <t xml:space="preserve">Penalty costs for absolute difference between tap positions of two time steps (gradients of tap position --&gt;Smooting the initial sequence _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_of tap positions</t>
   </si>
   <si>
     <t xml:space="preserve">Penalty Cost Delta RA (EUR/Delta tap h)</t>
@@ -1479,7 +1479,7 @@
     <t xml:space="preserve">15.02.2017</t>
   </si>
   <si>
-    <t xml:space="preserve">BBE1AA1  BBE2AA1  1</t>
+    <t xml:space="preserve">pstExample</t>
   </si>
   <si>
     <t xml:space="preserve">BBE2AA1 </t>
@@ -8011,7 +8011,7 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -10950,7 +10950,7 @@
     <tabColor rgb="FF9BBB59"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11660,34 +11660,6 @@
       <c r="A111" s="113"/>
       <c r="C111" s="105"/>
       <c r="K111" s="105"/>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="113"/>
-      <c r="C112" s="105"/>
-      <c r="G112" s="105"/>
-      <c r="K112" s="105"/>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="109"/>
-      <c r="C113" s="105"/>
-      <c r="G113" s="105"/>
-      <c r="K113" s="105"/>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="113"/>
-      <c r="C114" s="105"/>
-      <c r="G114" s="105"/>
-      <c r="K114" s="105"/>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="109"/>
-      <c r="C115" s="105"/>
-      <c r="G115" s="105"/>
-      <c r="K115" s="105"/>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="113"/>
-      <c r="C116" s="105"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A249:A1048576 A64:A87 A114 A116:A139 A141:A149 A151 A153:A161 A163:A170 A172:A210 A212:A217 A219:A247 A90:A112 A1:A62">
@@ -11831,7 +11803,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C92 G2:G116 K2:K116 C94:C116" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C92 G2:G111 K2:K111 C94:C111" type="list">
       <formula1>Elementdescriptionmode</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12547,8 +12519,8 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Debug crac xlsx pst import (#41)
* Correction of branch and generator id at import crac xlsx
</commit_message>
<xml_diff>
--- a/data/crac-file/crac-file-xlsx-api/src/test/resources/test_crac_simple.xlsx
+++ b/data/crac-file/crac-file-xlsx-api/src/test/resources/test_crac_simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">Penalty Cost Tap Change (EUR/Delta tap h)</t>
   </si>
   <si>
-    <t xml:space="preserve">Penalty costs for absolute difference between tap positions of two time steps (gradients of tap position --&gt;Smooting the initial sequence _x005F_x005F_x005F_x005F_x000B_of tap positions</t>
+    <t xml:space="preserve">Penalty costs for absolute difference between tap positions of two time steps (gradients of tap position --&gt;Smooting the initial sequence _x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_of tap positions</t>
   </si>
   <si>
     <t xml:space="preserve">Penalty Cost Delta RA (EUR/Delta tap h)</t>
@@ -1479,7 +1479,7 @@
     <t xml:space="preserve">15.02.2017</t>
   </si>
   <si>
-    <t xml:space="preserve">BBE1AA1  BBE2AA1  1</t>
+    <t xml:space="preserve">pstExample</t>
   </si>
   <si>
     <t xml:space="preserve">BBE2AA1 </t>
@@ -8011,7 +8011,7 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -10950,7 +10950,7 @@
     <tabColor rgb="FF9BBB59"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11660,34 +11660,6 @@
       <c r="A111" s="113"/>
       <c r="C111" s="105"/>
       <c r="K111" s="105"/>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="113"/>
-      <c r="C112" s="105"/>
-      <c r="G112" s="105"/>
-      <c r="K112" s="105"/>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="109"/>
-      <c r="C113" s="105"/>
-      <c r="G113" s="105"/>
-      <c r="K113" s="105"/>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="113"/>
-      <c r="C114" s="105"/>
-      <c r="G114" s="105"/>
-      <c r="K114" s="105"/>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="109"/>
-      <c r="C115" s="105"/>
-      <c r="G115" s="105"/>
-      <c r="K115" s="105"/>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="113"/>
-      <c r="C116" s="105"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A249:A1048576 A64:A87 A114 A116:A139 A141:A149 A151 A153:A161 A163:A170 A172:A210 A212:A217 A219:A247 A90:A112 A1:A62">
@@ -11831,7 +11803,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C92 G2:G116 K2:K116 C94:C116" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C92 G2:G111 K2:K111 C94:C111" type="list">
       <formula1>Elementdescriptionmode</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12547,8 +12519,8 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>